<commit_message>
This is direct commit
</commit_message>
<xml_diff>
--- a/excel1.xlsx
+++ b/excel1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dxcportal-my.sharepoint.com/personal/birendra_kumar3_dxc_com/Documents/Documents/github/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_F25DC773A252ABDACC10487F119971905ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A3CD1D8-E148-4D68-B85B-5225352B2895}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_F25DC773A252ABDACC10487F119971905ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75F51DE2-C86F-4986-9845-EE2F55EE592D}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="1">
   <si>
     <t>version6</t>
   </si>
@@ -345,9 +345,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -356,6 +358,16 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>